<commit_message>
Add sphinx gallery for all examples
- Remove attributes planning_im and applicant_ru (not needed for the model)
- route planning process now informs IMs after route redesign
- increment version after after first presentation of the model
</commit_message>
<xml_diff>
--- a/docs/examples/train-TR-13AB-1.xlsx
+++ b/docs/examples/train-TR-13AB-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\tap-tsi\fte-tom\tom\docs\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB2CE49-5E9F-4FF9-A62E-7A4DED39C5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A819D1AA-3B1D-4E66-8AD5-EFBF8E07C154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="164">
   <si>
     <t>Departure A</t>
   </si>
@@ -509,13 +509,16 @@
   </si>
   <si>
     <t>Fri 01.01.21 04:30  1</t>
+  </si>
+  <si>
+    <t>Daily Train ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,13 +538,26 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -571,12 +587,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -882,7 +903,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C14" sqref="A13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -893,6 +914,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1011,10 +1035,11 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1034,12 +1059,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>34</v>
       </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1172,10 +1198,11 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1195,12 +1222,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="C14" s="5"/>
       <c r="D14" s="1" t="s">
         <v>70</v>
       </c>
@@ -1333,10 +1361,11 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1356,12 +1385,13 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="5" t="s">
         <v>104</v>
       </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="1" t="s">
         <v>105</v>
       </c>
@@ -1494,10 +1524,11 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5" t="s">
         <v>134</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1517,12 +1548,13 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="5" t="s">
         <v>139</v>
       </c>
+      <c r="C28" s="5"/>
       <c r="D28" s="1" t="s">
         <v>140</v>
       </c>

</xml_diff>